<commit_message>
fixed naming inconsistencies bugs
</commit_message>
<xml_diff>
--- a/examples/excel.xlsx
+++ b/examples/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\SINERGIA\ShipmentsExtractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SINERGIA\File2CSV\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828D6746-C0DA-4B89-997F-2AD50DBC7B44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525F6452-46A1-4B29-A99D-ADBF3130E089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet3" sheetId="2" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>ENTRECALLES</t>
   </si>
   <si>
-    <t>TRACKING ID MERCADO LIBRE</t>
-  </si>
-  <si>
     <t>DOMICILIO</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>f hgj fg</t>
+  </si>
+  <si>
+    <t>ID FLEX</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -513,7 +513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -525,7 +525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -537,7 +537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -549,7 +549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,17 +563,17 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -586,116 +586,116 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:J3 A1 C1:J1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>